<commit_message>
santoshkumbhalkar: task of v_and_hlookup
</commit_message>
<xml_diff>
--- a/vlookup_and_hlookup.xlsx
+++ b/vlookup_and_hlookup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\Excel\Day_12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FC7F00-1463-40AF-BB53-CE6C7FF4E79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD970448-F241-4706-BC16-EC1DF9F8F2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t xml:space="preserve">VLOOKUP </t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>HLOOKUP</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -483,7 +495,7 @@
   <dimension ref="D2:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="D5" sqref="D5:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,7 +642,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" ref="G7:G11" si="1">VLOOKUP(D8,L$5:M$11,2,FALSE)</f>
+        <f t="shared" ref="G8:G11" si="1">VLOOKUP(D8,L$5:M$11,2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="H8" s="5">
@@ -768,7 +780,7 @@
   <dimension ref="C1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,7 +831,7 @@
         <v>automotive sq, near tp road , 400001</v>
       </c>
       <c r="E4" s="5" t="str">
-        <f t="shared" ref="E4:I4" si="0">HLOOKUP(E3,$C14:$I16,2,FALSE)</f>
+        <f t="shared" ref="E4:H4" si="0">HLOOKUP(E3,$C14:$I16,2,FALSE)</f>
         <v>offline</v>
       </c>
       <c r="F4" s="5">

</xml_diff>